<commit_message>
Cleaning code and adding temp hash store for validation duplication prevention
</commit_message>
<xml_diff>
--- a/output/kpi_original.xlsx
+++ b/output/kpi_original.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,7 +603,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>The study was for the monotherapy treatment of major depressive disorder and did not achieve statistical significance on the primary endpoint (change from baseline in the 17-item Hamilton Depression Rating Scale total score at Day 15).</t>
+          <t>The study did not achieve statistical significance on the primary endpoint of change from baseline in the 17-item Hamilton Depression Rating Scale total score at Day 15, or on any secondary endpoints.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Did not meet any secondary endpoints.</t>
+          <t>Did not meet any secondary endpoints</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Efficacy and safety</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0001689548-22-000038</t>
+          <t>0001689548-22-000111</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>In April 2022, the Investigational New Drug (IND) application for the study of PRAX-222 was placed on clinical hold by the FDA. The company had not received the full details on the reasons for the hold at the time of the report.</t>
+          <t>In April 2022, the Investigational New Drug application for the study of PRAX-222 was placed on clinical hold by the FDA. The company later submitted additional documentation from a toxicology study to address the hold.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>clinical hold</t>
+          <t>Clinical Hold</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Investigational New Drug application</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -795,7 +795,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Essential3 (Study 1 and Study 2)</t>
+          <t>Essential3 clinical program (Study 1 and Study 2)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>In February 2025, a pre-planned interim analysis of Study 1 resulted in the IDMC recommending the study be stopped for futility. The IDMC noted that underlying assumptions of the statistical model might have influenced this outcome. Given the advanced enrollment in both studies and the IDMC's advice, the company decided to continue both studies to completion. A decision on an NDA submission will be made after the final results are analyzed.</t>
+          <t>Based on a pre-planned interim analysis, the IDMC recommended that Study 1 be stopped for futility, as it was unlikely to meet the primary efficacy endpoint. The company has decided to continue both Study 1 and Study 2 to completion.</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>NDA</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0001689548-24-000101</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>epilepsy</t>
+          <t>Epilepsy</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Photo-Paroxysmal Response study</t>
+          <t>Photo-Paroxysmal Response (PPR) study</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Announced positive results from the Photo-Paroxysmal Response (PPR) study in the first quarter of 2024.</t>
+          <t>Announced positive results from the PPR study, which is part of the ENERGY program.</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>The RADIANT study is an open-label eight-week study that is part of the ENERGY program.</t>
+          <t>The RADIANT study is an open label eight-week study in patients with focal onset seizures or generalized epilepsy and is part of the ENERGY program.</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>The POWER 1 study is a double-blind, placebo-controlled, 12-week study in focal onset seizures.</t>
+          <t>The POWER 1 study is a 12-week study in focal onset seizures and is part of the ENERGY program.</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>double-blind, placebo-controlled, 12-week</t>
+          <t>double-blind, placebo-controlled</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>placebo</t>
+          <t>Placebo</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>epilepsy</t>
+          <t>Epilepsy</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1330,12 +1330,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>2025H2</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>The company plans to begin enrollment in the POWER 2 study, a third efficacy study, in the second half of 2025.</t>
+          <t>The POWER 2 study is the third efficacy study in the ENERGY program, with enrollment planned to begin in the second half of 2025.</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0001689548-24-000101</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>EMBOLD (first cohort)</t>
+          <t>EMBOLD study (first cohort)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>EMBOLD (second cohort)</t>
+          <t>EMBOLD study (second cohort)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>developmental and epileptic encephalopathies</t>
+          <t>developmental and epileptic encephalopathies (DEE)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>EMERALD</t>
+          <t>EMERALD study</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>The company plans to initiate the EMERALD study in a broader developmental and epileptic encephalopathies (DEE) patient population.</t>
+          <t>Plan to initiate the EMERALD study in a broader developmental and epileptic encephalopathies (DEE) patient population in mid-2025.</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0001689548-24-000101</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>EMBRAVE (Part 1)</t>
+          <t>EMBRAVE study (second cohort)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1813,17 +1813,17 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Announced</t>
+          <t>Expected</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2023Q4</t>
+          <t>2026H1</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Results from Part 1 of the EMBRAVE study were shared in the fourth quarter of 2023.</t>
+          <t>Currently enrolling the second cohort of the EMBRAVE study in Brazil, with topline results expected in the first half of 2026. Results from Part 1 were shared in the fourth quarter of 2023.</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1888,132 +1888,10 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Topline</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Praxis Precision Medicines Inc</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>0001689548-25-000058</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>elsunersen</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Pivotal Phase</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>EMBRAVE (second cohort)</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Expected</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2026H1</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>The second cohort of the EMBRAVE study is currently enrolling in Brazil. The company is also completing multiple global regulatory interactions to further expand the pivotal phase of the program.</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Brazil</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>Topline</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
         <is>
           <t>Enrolling</t>
         </is>

</xml_diff>